<commit_message>
Lidando com números repetidos
</commit_message>
<xml_diff>
--- a/TESTE.xlsx
+++ b/TESTE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">BA</t>
   </si>
@@ -55,6 +55,27 @@
     <t xml:space="preserve">03.004-000</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5511913592962;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5511913592962</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">(A)DIEGO DOS SANTOS NEVES</t>
   </si>
   <si>
@@ -64,6 +85,9 @@
     <t xml:space="preserve">03.007-040</t>
   </si>
   <si>
+    <t xml:space="preserve">5511913592962;5511913592962</t>
+  </si>
+  <si>
     <t xml:space="preserve">(A)CAROLINA KETYLLEN DA SILVA ZACARIAS</t>
   </si>
   <si>
@@ -71,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">03.009-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5511913592962;5511940280229</t>
   </si>
   <si>
     <t xml:space="preserve">BOX:3</t>
@@ -101,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -123,6 +150,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,7 +205,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,14 +229,14 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.14"/>
@@ -237,7 +270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>50425698</v>
       </c>
@@ -253,8 +286,8 @@
       <c r="E2" s="0" t="n">
         <v>144</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>5511913592962</v>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,19 +295,19 @@
         <v>50425595</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>322</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>5511913592962</v>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,22 +315,22 @@
         <v>50424816</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>696</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>5511913592962</v>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -305,13 +338,13 @@
         <v>50426350</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>127</v>
@@ -325,13 +358,13 @@
         <v>50425701</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>528</v>

</xml_diff>

<commit_message>
tornando a aplicação executavel
</commit_message>
<xml_diff>
--- a/TESTE.xlsx
+++ b/TESTE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">BA</t>
   </si>
@@ -55,25 +55,7 @@
     <t xml:space="preserve">03.004-000</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">5511913592962;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">5511913592962</t>
-    </r>
+    <t xml:space="preserve">5511913592962;5511913592962</t>
   </si>
   <si>
     <t xml:space="preserve">(A)DIEGO DOS SANTOS NEVES</t>
@@ -83,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">03.007-040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5511913592962;5511913592962</t>
   </si>
   <si>
     <t xml:space="preserve">(A)CAROLINA KETYLLEN DA SILVA ZACARIAS</t>
@@ -128,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,12 +129,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,7 +280,7 @@
         <v>322</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,22 +288,22 @@
         <v>50424816</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>696</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -338,13 +311,13 @@
         <v>50426350</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>127</v>
@@ -358,13 +331,13 @@
         <v>50425701</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>528</v>

</xml_diff>